<commit_message>
OSA03 Multi Filter Test cases
</commit_message>
<xml_diff>
--- a/InputFiles/TC05_Canine_StudyOSA03-Biobank_Breed_NeuteredStatus.xlsx
+++ b/InputFiles/TC05_Canine_StudyOSA03-Biobank_Breed_NeuteredStatus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\AutomationICDC\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608015D4-3758-4EFC-AB25-A762EEF07DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75514403-890A-4BA4-A7F7-99FB58CA1878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -60,19 +60,18 @@
     <t>StudyFilesTab</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;--(c:case)
-WHERE s.clinical_study_designation IN ['OSA01']
-MATCH (c)&lt;--(r:registration)
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE s.clinical_study_designation IN ['OSA03'] and demo.breed in ['Mastiff','Golden Retriever'] and demo.neutered_indicator in ['Yes']
+OPTIONAL MATCH (c)&lt;--(r:registration)
 WITH s, c, COLLECT(CASE r.registration_origin WHEN s.clinical_study_designation THEN null ELSE r.registration_origin END) AS registrations
 WHERE registrations = []
-MATCH (c)&lt;--(demo:demographic)
-Where demo.breed in ['Bullmastiff', 'Golden Retriever'] and demo.neutered_indicator in ['Yes']
 OPTIONAL MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (c)--&gt;(co:cohort)
-WITH c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
-RETURN coalesce(c.case_id, '') AS `Case ID` ,
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+OPTIONAL MATCH (c)&lt;--(demo:demographic)
+WITH DISTINCT c, s, demo, diag, co,demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
         coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS `Study Type`,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
         coalesce(demo.breed, '') AS Breed ,
         coalesce(diag.disease_term, '') AS Diagnosis ,
         coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
@@ -86,14 +85,39 @@
 limit 100</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-MATCH (r:registration)--&gt;(c)
-WHERE s.clinical_study_designation IN ['OSA01']
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE s.clinical_study_designation IN ['OSA03'] and demo.breed in ['Mastiff','Golden Retriever'] and demo.neutered_indicator in ['Yes']
+OPTIONAL MATCH (r:registration)--&gt;(c)
+WITH s, c, COLLECT(CASE r.registration_origin WHEN s.clinical_study_designation THEN null ELSE r.registration_origin END) AS registrations
+WHERE registrations = []
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (c)&lt;--(demo:demographic)
+OPTIONAL MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE s.clinical_study_designation IN ['OSA03'] and demo.breed in ['Mastiff','Golden Retriever'] and demo.neutered_indicator in ['Yes']
+OPTIONAL MATCH (r:registration)--&gt;(c)
 WITH s, c, COLLECT(CASE r.registration_origin WHEN s.clinical_study_designation THEN null ELSE r.registration_origin END) AS registrations
 WHERE registrations = []
 MATCH (f:file)--&gt;(parent)
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-Where demo.breed in ['Bullmastiff', 'Golden Retriever'] and demo.neutered_indicator in ['Yes']
 MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
 WITH
@@ -124,15 +148,13 @@
         limit 100</t>
   </si>
   <si>
-    <t>MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
-MATCH (r:registration)--&gt;(c)
-MATCH (c)&lt;--(demo:demographic)
-WHERE s.clinical_study_designation IN ['OSA01'] 
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE s.clinical_study_designation IN ['OSA03'] and demo.breed in ['Mastiff','Golden Retriever'] and demo.neutered_indicator in ['Yes']
+OPTIONAL MATCH (r:registration)--&gt;(c)
 WITH s, c, COLLECT(CASE r.registration_origin WHEN s.clinical_study_designation THEN null ELSE r.registration_origin END) AS registrations
 WHERE registrations = []
 MATCH (f:file)--&gt;(s:study)
 MATCH (c)&lt;--(demo:demographic)
-Where demo.breed in ['Bullmastiff', 'Golden Retriever'] and demo.neutered_indicator in ['Yes']
 MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
 WITH
         DISTINCT f, c, demo, diag, s,
@@ -158,19 +180,15 @@
   limit 100</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;--(c:case)
-MATCH (r:registration)--&gt;(c)
-WHERE s.clinical_study_designation IN ['OSA01']
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE s.clinical_study_designation IN ['OSA03'] and demo.breed in ['Mastiff','Golden Retriever'] and demo.neutered_indicator in ['Yes']
+OPTIONAL MATCH (c)&lt;--(r:registration)
 WITH s, c, COLLECT(CASE r.registration_origin WHEN s.clinical_study_designation THEN null ELSE r.registration_origin END) AS registrations
 WHERE registrations = []
-MATCH (c)&lt;--(demo:demographic)
-Where demo.breed in ['Bullmastiff', 'Golden Retriever'] and demo.neutered_indicator in ['Yes']
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (cf:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
 OPTIONAL MATCH (s)--&gt;(p:program)
-OPTIONAL MATCH (cf:file)-[*]-&gt;(c)
-OPTIONAL MATCH (p:program)--&gt;(s)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-OPTIONAL MATCH (c)--&gt;(co:cohort)
 RETURN
 	count(distinct p) AS Programs,
     count(distinct s) AS Studies,
@@ -184,32 +202,6 @@
   </si>
   <si>
     <t>TC05_Canine_StudyOSA03-Biobank_Breed_NeuteredStatus_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(c:case)
-WHERE s.clinical_study_designation IN ['OSA01']
-MATCH (c)&lt;--(r:registration)
-WITH s, c, COLLECT(CASE r.registration_origin WHEN s.clinical_study_designation THEN null ELSE r.registration_origin END) AS registrations
-WHERE registrations = []
-MATCH (c)&lt;--(demo:demographic)
-Where demo.breed in ['Great Pyrenees', 'Golden Retriever'] and demo.neutered_indicator in ['Yes']
-OPTIONAL MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed,
-        coalesce(diag.disease_term,'') AS Diagnosis, 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
-order by samp.sample_id asc
-limit 100</t>
   </si>
 </sst>
 </file>
@@ -279,10 +271,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -609,7 +601,7 @@
     <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
     <col min="2" max="3" width="75.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="70.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="92.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -637,14 +629,14 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -652,16 +644,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -669,33 +661,33 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="99.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>